<commit_message>
added mean squared error values to final answers gpom
</commit_message>
<xml_diff>
--- a/presentation/models.xlsx
+++ b/presentation/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddfloww/Documents/_datasci/Github/codeup-ds-projects/presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1957FB07-5DBE-024C-AB72-0F1EE38DA7DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C347063A-830F-974A-9939-F50A9318A577}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{ABD91C3E-A360-2848-8706-7CB331435585}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>'calculatedfinishedsquarefeet'</t>
   </si>
@@ -55,13 +55,19 @@
   </si>
   <si>
     <t>'airconditioningtypeid', 'heatingorsystemtypeid'</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>R^2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +78,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,23 +114,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,79 +479,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BF9150-9879-D246-BB5C-274753BF3C63}">
-  <dimension ref="E7:F14"/>
+  <dimension ref="E6:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="54.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:6" ht="22">
-      <c r="E7" s="2" t="s">
+    <row r="6" spans="5:7" ht="25">
+      <c r="E6" s="3"/>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" ht="22">
+      <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
+        <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="G7" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="5:6" ht="22">
-      <c r="E8" s="2" t="s">
+    <row r="8" spans="5:7" ht="22">
+      <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
+        <v>8.5599999999999999E-3</v>
+      </c>
+      <c r="G8" s="7">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="5:6" ht="22">
-      <c r="E9" s="2" t="s">
+    <row r="9" spans="5:7" ht="22">
+      <c r="E9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
+        <v>8.5900000000000004E-3</v>
+      </c>
+      <c r="G9" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="5:6" ht="66">
-      <c r="E10" s="2" t="s">
+    <row r="10" spans="5:7" ht="66">
+      <c r="E10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="10">
+        <v>8.4899999999999993E-3</v>
+      </c>
+      <c r="G10" s="7">
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="11" spans="5:6" ht="23" customHeight="1">
-      <c r="E11" s="2" t="s">
+    <row r="11" spans="5:7" ht="44">
+      <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
+        <v>8.5500000000000003E-3</v>
+      </c>
+      <c r="G11" s="7">
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="12" spans="5:6" ht="44">
-      <c r="E12" s="4" t="s">
+    <row r="12" spans="5:7" ht="44">
+      <c r="E12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="8">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="G12" s="9">
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="5:6" ht="22">
-      <c r="E13" s="2" t="s">
+    <row r="13" spans="5:7" ht="22">
+      <c r="E13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="G13" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="5:6" ht="44">
-      <c r="E14" s="2" t="s">
+    <row r="14" spans="5:7" ht="44">
+      <c r="E14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="G14" s="7">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>

</xml_diff>